<commit_message>
RESUBMIT the Case Study - Customer Segmentation using Clustering: K-means from unit 15.6.3
</commit_message>
<xml_diff>
--- a/Unit 15 - Unsupervised Learning/15.6 Principal Components Analysis/Clustering Case Study Customer Segmentation/WineKMC.xlsx
+++ b/Unit 15 - Unsupervised Learning/15.6 Principal Components Analysis/Clustering Case Study Customer Segmentation/WineKMC.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Farid\gitProjects\Springboard\Unit 15 - Unsupervised Learning\15.6 Principal Components Analysis\Clustering Case Study Customer Segmentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{38B91296-FF11-486D-8CCE-27A28074E263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="871" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="871" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OfferInformation" sheetId="49" r:id="rId1"/>
@@ -448,7 +454,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1043,6 +1049,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1367,21 +1381,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>138</v>
       </c>
@@ -1404,7 +1418,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1427,7 +1441,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1450,7 +1464,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1473,7 +1487,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1496,7 +1510,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1519,7 +1533,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1542,7 +1556,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1565,7 +1579,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1588,7 +1602,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1611,7 +1625,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1634,7 +1648,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1657,7 +1671,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1680,7 +1694,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1703,7 +1717,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1726,7 +1740,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1749,7 +1763,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1772,7 +1786,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1795,7 +1809,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1818,7 +1832,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1841,7 +1855,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1864,7 +1878,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1887,7 +1901,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1910,7 +1924,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1933,7 +1947,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1956,7 +1970,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1979,7 +1993,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2002,7 +2016,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2025,7 +2039,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2048,7 +2062,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2071,7 +2085,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2094,7 +2108,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2117,7 +2131,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2152,18 +2166,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B325"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>139</v>
       </c>
@@ -2171,7 +2185,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2179,7 +2193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2187,7 +2201,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2195,7 +2209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2203,7 +2217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2211,7 +2225,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2219,7 +2233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2227,7 +2241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2235,7 +2249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2243,7 +2257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2251,7 +2265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2259,7 +2273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2267,7 +2281,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2275,7 +2289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2283,7 +2297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2291,7 +2305,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2299,7 +2313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2307,7 +2321,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2315,7 +2329,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2323,7 +2337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2331,7 +2345,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2339,7 +2353,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -2347,7 +2361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -2355,7 +2369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -2363,7 +2377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -2371,7 +2385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -2379,7 +2393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2387,7 +2401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2395,7 +2409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -2403,7 +2417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2411,7 +2425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2419,7 +2433,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2427,7 +2441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2435,7 +2449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2443,7 +2457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2451,7 +2465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2459,7 +2473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2467,7 +2481,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2475,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2483,7 +2497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2491,7 +2505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2499,7 +2513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2507,7 +2521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2515,7 +2529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -2523,7 +2537,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -2531,7 +2545,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2539,7 +2553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2547,7 +2561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2555,7 +2569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2563,7 +2577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -2571,7 +2585,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2579,7 +2593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2587,7 +2601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2595,7 +2609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -2603,7 +2617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -2611,7 +2625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -2619,7 +2633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -2627,7 +2641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -2635,7 +2649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -2643,7 +2657,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -2651,7 +2665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -2659,7 +2673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -2667,7 +2681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -2675,7 +2689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>98</v>
       </c>
@@ -2683,7 +2697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -2691,7 +2705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>98</v>
       </c>
@@ -2699,7 +2713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>98</v>
       </c>
@@ -2707,7 +2721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>98</v>
       </c>
@@ -2715,7 +2729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -2723,7 +2737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -2731,7 +2745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -2739,7 +2753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -2747,7 +2761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -2755,7 +2769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -2763,7 +2777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -2771,7 +2785,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -2779,7 +2793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -2787,7 +2801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2795,7 +2809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2803,7 +2817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -2811,7 +2825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -2819,7 +2833,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>20</v>
       </c>
@@ -2827,7 +2841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -2835,7 +2849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -2843,7 +2857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -2851,7 +2865,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>21</v>
       </c>
@@ -2859,7 +2873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>21</v>
       </c>
@@ -2867,7 +2881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>21</v>
       </c>
@@ -2875,7 +2889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -2883,7 +2897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -2891,7 +2905,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>23</v>
       </c>
@@ -2899,7 +2913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>23</v>
       </c>
@@ -2907,7 +2921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -2915,7 +2929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>100</v>
       </c>
@@ -2923,7 +2937,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -2931,7 +2945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -2939,7 +2953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -2947,7 +2961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>25</v>
       </c>
@@ -2955,7 +2969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>25</v>
       </c>
@@ -2963,7 +2977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>25</v>
       </c>
@@ -2971,7 +2985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>25</v>
       </c>
@@ -2979,7 +2993,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>25</v>
       </c>
@@ -2987,7 +3001,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>26</v>
       </c>
@@ -2995,7 +3009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -3003,7 +3017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -3011,7 +3025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -3019,7 +3033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>97</v>
       </c>
@@ -3027,7 +3041,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -3035,7 +3049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>97</v>
       </c>
@@ -3043,7 +3057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -3051,7 +3065,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -3059,7 +3073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>27</v>
       </c>
@@ -3067,7 +3081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>27</v>
       </c>
@@ -3075,7 +3089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>27</v>
       </c>
@@ -3083,7 +3097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>27</v>
       </c>
@@ -3091,7 +3105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>28</v>
       </c>
@@ -3099,7 +3113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>28</v>
       </c>
@@ -3107,7 +3121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>28</v>
       </c>
@@ -3115,7 +3129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>28</v>
       </c>
@@ -3123,7 +3137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>29</v>
       </c>
@@ -3131,7 +3145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>29</v>
       </c>
@@ -3139,7 +3153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>29</v>
       </c>
@@ -3147,7 +3161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>30</v>
       </c>
@@ -3155,7 +3169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>31</v>
       </c>
@@ -3163,7 +3177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>31</v>
       </c>
@@ -3171,7 +3185,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>31</v>
       </c>
@@ -3179,7 +3193,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>31</v>
       </c>
@@ -3187,7 +3201,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>32</v>
       </c>
@@ -3195,7 +3209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>32</v>
       </c>
@@ -3203,7 +3217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>32</v>
       </c>
@@ -3211,7 +3225,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>33</v>
       </c>
@@ -3219,7 +3233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>33</v>
       </c>
@@ -3227,7 +3241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>33</v>
       </c>
@@ -3235,7 +3249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>33</v>
       </c>
@@ -3243,7 +3257,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>34</v>
       </c>
@@ -3251,7 +3265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>34</v>
       </c>
@@ -3259,7 +3273,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -3267,7 +3281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>34</v>
       </c>
@@ -3275,7 +3289,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>93</v>
       </c>
@@ -3283,7 +3297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>35</v>
       </c>
@@ -3291,7 +3305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>35</v>
       </c>
@@ -3299,7 +3313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>35</v>
       </c>
@@ -3307,7 +3321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>36</v>
       </c>
@@ -3315,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>36</v>
       </c>
@@ -3323,7 +3337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>37</v>
       </c>
@@ -3331,7 +3345,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>38</v>
       </c>
@@ -3339,7 +3353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>38</v>
       </c>
@@ -3347,7 +3361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>38</v>
       </c>
@@ -3355,7 +3369,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>38</v>
       </c>
@@ -3363,7 +3377,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>39</v>
       </c>
@@ -3371,7 +3385,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>39</v>
       </c>
@@ -3379,7 +3393,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>40</v>
       </c>
@@ -3387,7 +3401,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>40</v>
       </c>
@@ -3395,7 +3409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>41</v>
       </c>
@@ -3403,7 +3417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>41</v>
       </c>
@@ -3411,7 +3425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>41</v>
       </c>
@@ -3419,7 +3433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>41</v>
       </c>
@@ -3427,7 +3441,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -3435,7 +3449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>43</v>
       </c>
@@ -3443,7 +3457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>43</v>
       </c>
@@ -3451,7 +3465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>43</v>
       </c>
@@ -3459,7 +3473,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>43</v>
       </c>
@@ -3467,7 +3481,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>43</v>
       </c>
@@ -3475,7 +3489,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>44</v>
       </c>
@@ -3483,7 +3497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>44</v>
       </c>
@@ -3491,7 +3505,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>45</v>
       </c>
@@ -3499,7 +3513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>45</v>
       </c>
@@ -3507,7 +3521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>46</v>
       </c>
@@ -3515,7 +3529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>46</v>
       </c>
@@ -3523,7 +3537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -3531,7 +3545,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>47</v>
       </c>
@@ -3539,7 +3553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>47</v>
       </c>
@@ -3547,7 +3561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -3555,7 +3569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -3563,7 +3577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -3571,7 +3585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>49</v>
       </c>
@@ -3579,7 +3593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>49</v>
       </c>
@@ -3587,7 +3601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>50</v>
       </c>
@@ -3595,7 +3609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>50</v>
       </c>
@@ -3603,7 +3617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>51</v>
       </c>
@@ -3611,7 +3625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>51</v>
       </c>
@@ -3619,7 +3633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>52</v>
       </c>
@@ -3627,7 +3641,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>52</v>
       </c>
@@ -3635,7 +3649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>53</v>
       </c>
@@ -3643,7 +3657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>53</v>
       </c>
@@ -3651,7 +3665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>53</v>
       </c>
@@ -3659,7 +3673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>53</v>
       </c>
@@ -3667,7 +3681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>53</v>
       </c>
@@ -3675,7 +3689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>53</v>
       </c>
@@ -3683,7 +3697,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>54</v>
       </c>
@@ -3691,7 +3705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>54</v>
       </c>
@@ -3699,7 +3713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>55</v>
       </c>
@@ -3707,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>55</v>
       </c>
@@ -3715,7 +3729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>55</v>
       </c>
@@ -3723,7 +3737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>55</v>
       </c>
@@ -3731,7 +3745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>55</v>
       </c>
@@ -3739,7 +3753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>55</v>
       </c>
@@ -3747,7 +3761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>56</v>
       </c>
@@ -3755,7 +3769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>56</v>
       </c>
@@ -3763,7 +3777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>56</v>
       </c>
@@ -3771,7 +3785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>56</v>
       </c>
@@ -3779,7 +3793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>57</v>
       </c>
@@ -3787,7 +3801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>57</v>
       </c>
@@ -3795,7 +3809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>58</v>
       </c>
@@ -3803,7 +3817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>58</v>
       </c>
@@ -3811,7 +3825,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>59</v>
       </c>
@@ -3819,7 +3833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>59</v>
       </c>
@@ -3827,7 +3841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>59</v>
       </c>
@@ -3835,7 +3849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>59</v>
       </c>
@@ -3843,7 +3857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>99</v>
       </c>
@@ -3851,7 +3865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>99</v>
       </c>
@@ -3859,7 +3873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>99</v>
       </c>
@@ -3867,7 +3881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>99</v>
       </c>
@@ -3875,7 +3889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>60</v>
       </c>
@@ -3883,7 +3897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>60</v>
       </c>
@@ -3891,7 +3905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>60</v>
       </c>
@@ -3899,7 +3913,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>60</v>
       </c>
@@ -3907,7 +3921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>61</v>
       </c>
@@ -3915,7 +3929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>61</v>
       </c>
@@ -3923,7 +3937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>61</v>
       </c>
@@ -3931,7 +3945,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>62</v>
       </c>
@@ -3939,7 +3953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>63</v>
       </c>
@@ -3947,7 +3961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>63</v>
       </c>
@@ -3955,7 +3969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>63</v>
       </c>
@@ -3963,7 +3977,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>63</v>
       </c>
@@ -3971,7 +3985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>94</v>
       </c>
@@ -3979,7 +3993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>94</v>
       </c>
@@ -3987,7 +4001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>94</v>
       </c>
@@ -3995,7 +4009,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>94</v>
       </c>
@@ -4003,7 +4017,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>64</v>
       </c>
@@ -4011,7 +4025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>64</v>
       </c>
@@ -4019,7 +4033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>64</v>
       </c>
@@ -4027,7 +4041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>65</v>
       </c>
@@ -4035,7 +4049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>65</v>
       </c>
@@ -4043,7 +4057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>65</v>
       </c>
@@ -4051,7 +4065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>65</v>
       </c>
@@ -4059,7 +4073,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>66</v>
       </c>
@@ -4067,7 +4081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>66</v>
       </c>
@@ -4075,7 +4089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>67</v>
       </c>
@@ -4083,7 +4097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>67</v>
       </c>
@@ -4099,7 +4113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>67</v>
       </c>
@@ -4107,7 +4121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>68</v>
       </c>
@@ -4115,7 +4129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>68</v>
       </c>
@@ -4123,7 +4137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>69</v>
       </c>
@@ -4131,7 +4145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>69</v>
       </c>
@@ -4139,7 +4153,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>69</v>
       </c>
@@ -4147,7 +4161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>70</v>
       </c>
@@ -4155,7 +4169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>70</v>
       </c>
@@ -4163,7 +4177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>70</v>
       </c>
@@ -4171,7 +4185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>70</v>
       </c>
@@ -4179,7 +4193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>70</v>
       </c>
@@ -4187,7 +4201,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>71</v>
       </c>
@@ -4195,7 +4209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>71</v>
       </c>
@@ -4203,7 +4217,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>72</v>
       </c>
@@ -4211,7 +4225,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>72</v>
       </c>
@@ -4219,7 +4233,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>73</v>
       </c>
@@ -4227,7 +4241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>73</v>
       </c>
@@ -4235,7 +4249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>73</v>
       </c>
@@ -4243,7 +4257,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>73</v>
       </c>
@@ -4251,7 +4265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>73</v>
       </c>
@@ -4259,7 +4273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>74</v>
       </c>
@@ -4267,7 +4281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>74</v>
       </c>
@@ -4275,7 +4289,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>74</v>
       </c>
@@ -4283,7 +4297,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>74</v>
       </c>
@@ -4291,7 +4305,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>75</v>
       </c>
@@ -4299,7 +4313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>75</v>
       </c>
@@ -4307,7 +4321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>76</v>
       </c>
@@ -4315,7 +4329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>76</v>
       </c>
@@ -4323,7 +4337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>76</v>
       </c>
@@ -4331,7 +4345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>77</v>
       </c>
@@ -4339,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>77</v>
       </c>
@@ -4347,7 +4361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>77</v>
       </c>
@@ -4355,7 +4369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>77</v>
       </c>
@@ -4363,7 +4377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>77</v>
       </c>
@@ -4371,7 +4385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>78</v>
       </c>
@@ -4379,7 +4393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>78</v>
       </c>
@@ -4387,7 +4401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>78</v>
       </c>
@@ -4395,7 +4409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>78</v>
       </c>
@@ -4403,7 +4417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>78</v>
       </c>
@@ -4411,7 +4425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>78</v>
       </c>
@@ -4419,7 +4433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>78</v>
       </c>
@@ -4427,7 +4441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>78</v>
       </c>
@@ -4435,7 +4449,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>78</v>
       </c>
@@ -4443,7 +4457,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>79</v>
       </c>
@@ -4451,7 +4465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>79</v>
       </c>
@@ -4459,7 +4473,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>80</v>
       </c>
@@ -4467,7 +4481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>80</v>
       </c>
@@ -4475,7 +4489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>80</v>
       </c>
@@ -4483,7 +4497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>80</v>
       </c>
@@ -4491,7 +4505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>80</v>
       </c>
@@ -4499,7 +4513,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>80</v>
       </c>
@@ -4507,7 +4521,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>81</v>
       </c>
@@ -4515,7 +4529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>82</v>
       </c>
@@ -4523,7 +4537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>82</v>
       </c>
@@ -4531,7 +4545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>82</v>
       </c>
@@ -4539,7 +4553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>83</v>
       </c>
@@ -4547,7 +4561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>84</v>
       </c>
@@ -4555,7 +4569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>85</v>
       </c>
@@ -4563,7 +4577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>85</v>
       </c>
@@ -4571,7 +4585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>101</v>
       </c>
@@ -4579,7 +4593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>101</v>
       </c>
@@ -4587,7 +4601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>101</v>
       </c>
@@ -4595,7 +4609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305" spans="1:2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>101</v>
       </c>
@@ -4603,7 +4617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="306" spans="1:2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>86</v>
       </c>
@@ -4611,7 +4625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="307" spans="1:2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>86</v>
       </c>
@@ -4619,7 +4633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="308" spans="1:2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>86</v>
       </c>
@@ -4627,7 +4641,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="309" spans="1:2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>86</v>
       </c>
@@ -4635,7 +4649,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="310" spans="1:2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>87</v>
       </c>
@@ -4643,7 +4657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>87</v>
       </c>
@@ -4651,7 +4665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>87</v>
       </c>
@@ -4659,7 +4673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="313" spans="1:2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>87</v>
       </c>
@@ -4667,7 +4681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>87</v>
       </c>
@@ -4675,7 +4689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>88</v>
       </c>
@@ -4683,7 +4697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>88</v>
       </c>
@@ -4691,7 +4705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>88</v>
       </c>
@@ -4699,7 +4713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>88</v>
       </c>
@@ -4707,7 +4721,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>89</v>
       </c>
@@ -4715,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>89</v>
       </c>
@@ -4723,7 +4737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>89</v>
       </c>
@@ -4731,7 +4745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>89</v>
       </c>
@@ -4739,7 +4753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>89</v>
       </c>
@@ -4747,7 +4761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>89</v>
       </c>
@@ -4755,7 +4769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>89</v>
       </c>

</xml_diff>